<commit_message>
Finished preparing burndown chart for second sprint
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint1/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\IdeaProjects\OliveiraGant\ganttproject\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65355C5F-D886-419A-809C-DD34A75930CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911DE4B7-7363-4EC4-B6B8-0A908A25E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Task ID</t>
   </si>
@@ -54,7 +54,22 @@
     <t>Ideal Burndown</t>
   </si>
   <si>
-    <t>Sprint 1 Burndown Chart</t>
+    <t>Sugerir 2 Features (Francisco)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (Iago)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (James)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (Joao)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (Ricardo)</t>
+  </si>
+  <si>
+    <t>Sprint 2 Burndown Chart</t>
   </si>
 </sst>
 </file>
@@ -150,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -437,11 +452,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -501,9 +540,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -559,6 +595,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -664,7 +709,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$11:$C$11</c:f>
+              <c:f>'Burndown Chart'!$B$18:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -685,7 +730,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$11:$K$11</c:f>
+              <c:f>'Burndown Chart'!$D$18:$K$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -743,7 +788,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$12:$C$12</c:f>
+              <c:f>'Burndown Chart'!$B$19:$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -810,33 +855,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$12:$K$12</c:f>
+              <c:f>'Burndown Chart'!$D$19:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -853,7 +898,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$13:$C$13</c:f>
+              <c:f>'Burndown Chart'!$B$20:$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -908,30 +953,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$13:$K$13</c:f>
+              <c:f>'Burndown Chart'!$D$20:$K$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.2857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.8571428571428572</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.1428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.4285714285714284</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.71428571428571441</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1768,13 +1813,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>16807</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>180414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>177054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2100,10 +2145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L13"/>
+  <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2111,72 +2156,74 @@
     <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="33"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="37" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>44849</v>
+        <v>44872</v>
       </c>
       <c r="F4" s="3">
-        <v>44850</v>
+        <v>44873</v>
       </c>
       <c r="G4" s="3">
-        <v>44851</v>
+        <v>44874</v>
       </c>
       <c r="H4" s="3">
-        <v>44852</v>
+        <v>44875</v>
       </c>
       <c r="I4" s="3">
-        <v>44853</v>
+        <v>44876</v>
       </c>
       <c r="J4" s="3">
-        <v>44854</v>
+        <v>44876</v>
       </c>
       <c r="K4" s="3">
-        <v>44855</v>
+        <v>44878</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="38"/>
-      <c r="C5" s="36"/>
+    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="37"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2202,12 +2249,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="20">
         <v>1</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="23"/>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -2216,12 +2267,16 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="22">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="21">
         <v>2</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="24"/>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="23">
+        <v>1</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -2230,12 +2285,16 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="22">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="21">
         <v>3</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="24"/>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="23">
+        <v>1</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -2244,12 +2303,16 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="22">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="21">
         <v>4</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="24"/>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="23">
+        <v>1</v>
+      </c>
       <c r="E9" s="10"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -2258,12 +2321,16 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="22">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="21">
         <v>5</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="25"/>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="24">
+        <v>1</v>
+      </c>
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -2272,129 +2339,206 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="28" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="40"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+    </row>
+    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="40"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="1">
+      <c r="C18" s="28"/>
+      <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="13">
-        <f t="shared" ref="E11:K11" si="0">SUM(E6:E10)</f>
+      <c r="E18" s="13">
+        <f>SUM(E6:E17)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="13">
-        <f t="shared" si="0"/>
+      <c r="F18" s="13">
+        <f>SUM(F6:F17)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="13">
-        <f t="shared" si="0"/>
+      <c r="G18" s="13">
+        <f>SUM(G6:G17)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="13">
-        <f t="shared" si="0"/>
+      <c r="H18" s="13">
+        <f>SUM(H6:H17)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="13">
-        <f t="shared" si="0"/>
+      <c r="I18" s="13">
+        <f>SUM(I6:I17)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="13">
-        <f t="shared" si="0"/>
+      <c r="J18" s="13">
+        <f>SUM(J6:J17)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="13">
-        <f t="shared" si="0"/>
+      <c r="K18" s="13">
+        <f>SUM(K6:K17)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="19"/>
+      <c r="L18" s="19"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="39" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="15">
-        <f>SUM(D6:D11)</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="16">
-        <f t="shared" ref="E12:K12" si="1">D12-SUM(E6:E10)</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C19" s="39"/>
+      <c r="D19" s="15">
+        <f>SUM(D6:D18)</f>
+        <v>5</v>
+      </c>
+      <c r="E19" s="16">
+        <f>D19-SUM(E6:E10)</f>
+        <v>5</v>
+      </c>
+      <c r="F19" s="14">
+        <f>E19-SUM(F6:F10)</f>
+        <v>5</v>
+      </c>
+      <c r="G19" s="14">
+        <f>F19-SUM(G6:G10)</f>
+        <v>5</v>
+      </c>
+      <c r="H19" s="14">
+        <f>G19-SUM(H6:H10)</f>
+        <v>5</v>
+      </c>
+      <c r="I19" s="14">
+        <f>H19-SUM(I6:I10)</f>
+        <v>5</v>
+      </c>
+      <c r="J19" s="12">
+        <f>I19-SUM(J6:J10)</f>
+        <v>5</v>
+      </c>
+      <c r="K19" s="12">
+        <f>J19-SUM(K6:K10)</f>
+        <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="26" t="s">
+    <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="17">
-        <f>D12</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="18">
-        <f>$D$13-($D$13/$K$5*E5)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
-        <f t="shared" ref="F13:K13" si="2">$D$13-($D$13/$K$5*F5)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
-        <f t="shared" si="2"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="17">
+        <f>D19</f>
+        <v>5</v>
+      </c>
+      <c r="E20" s="18">
+        <f>$D$20-($D$20/$K$5*E5)</f>
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="F20" s="18">
+        <f>$D$20-($D$20/$K$5*F5)</f>
+        <v>3.5714285714285712</v>
+      </c>
+      <c r="G20" s="18">
+        <f>$D$20-($D$20/$K$5*G5)</f>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="H20" s="18">
+        <f>$D$20-($D$20/$K$5*H5)</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="I20" s="18">
+        <f>$D$20-($D$20/$K$5*I5)</f>
+        <v>1.4285714285714284</v>
+      </c>
+      <c r="J20" s="18">
+        <f>$D$20-($D$20/$K$5*J5)</f>
+        <v>0.71428571428571441</v>
+      </c>
+      <c r="K20" s="18">
+        <f>$D$20-($D$20/$K$5*K5)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished first cycle of second sprint (Phase 1 Sprint 1)
Everyone has given their suggestions
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint1/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\IdeaProjects\OliveiraGant\ganttproject\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911DE4B7-7363-4EC4-B6B8-0A908A25E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E1E4A9-903D-4E0B-9A20-27AECF2BE392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Task ID</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Sprint 2 Burndown Chart</t>
+  </si>
+  <si>
+    <t>Criar User Story Primeira Feature</t>
+  </si>
+  <si>
+    <t>Criar User Story Segunda Feature</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -515,13 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -552,6 +552,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,15 +604,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -738,7 +738,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -860,28 +860,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,25 +958,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.2857142857142856</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5714285714285712</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8571428571428572</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1428571428571428</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4285714285714284</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.71428571428571441</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2148,7 +2148,7 @@
   <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2164,36 +2164,36 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="34"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2222,8 +2222,8 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="37"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2250,16 +2250,18 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="20">
         <v>1</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -2268,16 +2270,18 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="21">
         <v>1</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -2286,16 +2290,18 @@
       <c r="K7" s="8"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="21">
         <v>1</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -2304,16 +2310,18 @@
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="21">
+      <c r="B9" s="19">
         <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="21">
         <v>1</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -2322,16 +2330,18 @@
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="21">
+      <c r="B10" s="19">
         <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="22">
         <v>1</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="11">
+        <v>1</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -2340,193 +2350,213 @@
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
+      <c r="B11" s="23">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="24">
+        <v>1</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="40"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
+      <c r="B12" s="23">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
+      <c r="B13" s="23">
+        <v>8</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
+      <c r="B14" s="23">
+        <v>9</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="40"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
+      <c r="B15" s="23">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="40"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
+      <c r="B16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
+      <c r="B17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18" s="13">
-        <f>SUM(E6:E17)</f>
+      <c r="E18" s="12">
+        <f t="shared" ref="E18:K18" si="0">SUM(E6:E17)</f>
+        <v>5</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="13">
-        <f>SUM(F6:F17)</f>
+      <c r="G18" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="13">
-        <f>SUM(G6:G17)</f>
+      <c r="H18" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="13">
-        <f>SUM(H6:H17)</f>
+      <c r="I18" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="13">
-        <f>SUM(I6:I17)</f>
+      <c r="J18" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="13">
-        <f>SUM(J6:J17)</f>
+      <c r="K18" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="13">
-        <f>SUM(K6:K17)</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="19"/>
+      <c r="L18" s="17"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="15">
+      <c r="C19" s="40"/>
+      <c r="D19" s="13">
         <f>SUM(D6:D18)</f>
-        <v>5</v>
-      </c>
-      <c r="E19" s="16">
-        <f>D19-SUM(E6:E10)</f>
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E19" s="14">
+        <f>D19-E18</f>
+        <v>2</v>
       </c>
       <c r="F19" s="14">
-        <f>E19-SUM(F6:F10)</f>
-        <v>5</v>
+        <f t="shared" ref="F19:K19" si="1">E19-F18</f>
+        <v>2</v>
       </c>
       <c r="G19" s="14">
-        <f>F19-SUM(G6:G10)</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="H19" s="14">
-        <f>G19-SUM(H6:H10)</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I19" s="14">
-        <f>H19-SUM(I6:I10)</f>
-        <v>5</v>
-      </c>
-      <c r="J19" s="12">
-        <f>I19-SUM(J6:J10)</f>
-        <v>5</v>
-      </c>
-      <c r="K19" s="12">
-        <f>J19-SUM(K6:K10)</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="17">
+      <c r="C20" s="27"/>
+      <c r="D20" s="15">
         <f>D19</f>
+        <v>7</v>
+      </c>
+      <c r="E20" s="14">
+        <f>D20-E19</f>
         <v>5</v>
       </c>
-      <c r="E20" s="18">
-        <f>$D$20-($D$20/$K$5*E5)</f>
-        <v>4.2857142857142856</v>
-      </c>
-      <c r="F20" s="18">
-        <f>$D$20-($D$20/$K$5*F5)</f>
-        <v>3.5714285714285712</v>
-      </c>
-      <c r="G20" s="18">
-        <f>$D$20-($D$20/$K$5*G5)</f>
-        <v>2.8571428571428572</v>
-      </c>
-      <c r="H20" s="18">
-        <f>$D$20-($D$20/$K$5*H5)</f>
-        <v>2.1428571428571428</v>
-      </c>
-      <c r="I20" s="18">
-        <f>$D$20-($D$20/$K$5*I5)</f>
-        <v>1.4285714285714284</v>
-      </c>
-      <c r="J20" s="18">
-        <f>$D$20-($D$20/$K$5*J5)</f>
-        <v>0.71428571428571441</v>
-      </c>
-      <c r="K20" s="18">
-        <f>$D$20-($D$20/$K$5*K5)</f>
+      <c r="F20" s="16">
+        <f t="shared" ref="E20:K20" si="2">$D$20-($D$20/$K$5*F5)</f>
+        <v>5</v>
+      </c>
+      <c r="G20" s="16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H20" s="16">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J20" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="16">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished second cycle of the second sprint (Sprint 1 Phase 2)
Features e User Stories usadas para faar com o professor em aula
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint1/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\IdeaProjects\OliveiraGant\ganttproject\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E1E4A9-903D-4E0B-9A20-27AECF2BE392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BC0B90-DC51-4663-8561-ED027D615997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Task ID</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Criar User Story Segunda Feature</t>
+  </si>
+  <si>
+    <t>Descrever Totalmente Primeita Feature</t>
+  </si>
+  <si>
+    <t>Descrever Totalmente Segunda Feature</t>
   </si>
 </sst>
 </file>
@@ -741,7 +747,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -860,28 +866,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>7</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,25 +964,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>7</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7.8571428571428577</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>6.2857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4.7142857142857144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3.1428571428571432</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2148,7 +2154,7 @@
   <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2360,7 +2366,9 @@
         <v>1</v>
       </c>
       <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="F11" s="25">
+        <v>1</v>
+      </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
@@ -2378,7 +2386,9 @@
         <v>1</v>
       </c>
       <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -2389,7 +2399,12 @@
       <c r="B13" s="23">
         <v>8</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="24">
+        <v>2</v>
+      </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -2402,7 +2417,12 @@
       <c r="B14" s="23">
         <v>9</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="24">
+        <v>2</v>
+      </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -2460,7 +2480,7 @@
       </c>
       <c r="F18" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="12">
         <f t="shared" si="0"/>
@@ -2491,35 +2511,35 @@
       <c r="C19" s="40"/>
       <c r="D19" s="13">
         <f>SUM(D6:D18)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E19" s="14">
         <f>D19-E18</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F19" s="14">
         <f t="shared" ref="F19:K19" si="1">E19-F18</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G19" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H19" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I19" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K19" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2529,7 +2549,7 @@
       <c r="C20" s="27"/>
       <c r="D20" s="15">
         <f>D19</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E20" s="14">
         <f>D20-E19</f>
@@ -2537,23 +2557,23 @@
       </c>
       <c r="F20" s="16">
         <f t="shared" ref="E20:K20" si="2">$D$20-($D$20/$K$5*F5)</f>
-        <v>5</v>
+        <v>7.8571428571428577</v>
       </c>
       <c r="G20" s="16">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6.2857142857142856</v>
       </c>
       <c r="H20" s="16">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4.7142857142857144</v>
       </c>
       <c r="I20" s="16">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3.1428571428571432</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.5714285714285712</v>
       </c>
       <c r="K20" s="16">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Finished third cycle of second sprint (Sprint 1 Phase 2)
Completely defined features to implement
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint1/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\IdeaProjects\OliveiraGant\ganttproject\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BC0B90-DC51-4663-8561-ED027D615997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C8EAE6-7C38-450C-906B-9E3F432A43A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -750,10 +750,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -875,19 +875,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -967,7 +967,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>9.4285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7.8571428571428577</c:v>
@@ -2154,7 +2154,7 @@
   <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2407,8 +2407,12 @@
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="25">
+        <v>1</v>
+      </c>
+      <c r="H13" s="25">
+        <v>1</v>
+      </c>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
@@ -2425,8 +2429,12 @@
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="G14" s="25">
+        <v>1</v>
+      </c>
+      <c r="H14" s="25">
+        <v>1</v>
+      </c>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
@@ -2484,11 +2492,11 @@
       </c>
       <c r="G18" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="12">
         <f t="shared" si="0"/>
@@ -2523,23 +2531,23 @@
       </c>
       <c r="G19" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I19" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K19" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2551,12 +2559,12 @@
         <f>D19</f>
         <v>11</v>
       </c>
-      <c r="E20" s="14">
-        <f>D20-E19</f>
-        <v>5</v>
+      <c r="E20" s="16">
+        <f t="shared" ref="E20:K20" si="2">$D$20-($D$20/$K$5*E5)</f>
+        <v>9.4285714285714288</v>
       </c>
       <c r="F20" s="16">
-        <f t="shared" ref="E20:K20" si="2">$D$20-($D$20/$K$5*F5)</f>
+        <f t="shared" si="2"/>
         <v>7.8571428571428577</v>
       </c>
       <c r="G20" s="16">

</xml_diff>